<commit_message>
Revert "4445 - Часть 2"
</commit_message>
<xml_diff>
--- a/Source/Libraries/Core/Business/Vodovoz.Reports/Reports/Sales/TurnoverReport.xlsx
+++ b/Source/Libraries/Core/Business/Vodovoz.Reports/Reports/Sales/TurnoverReport.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rm87\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{701E2721-ACDE-4BC0-B762-BA047BD8D393}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3473DB2F-0590-41B2-B501-B9D44D181174}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3945" yWindow="4260" windowWidth="21555" windowHeight="11340" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ReportTotal_SliceColumnValues">Sheet1!$E$9</definedName>
-    <definedName name="Rows">Sheet1!$A$11:$I$12</definedName>
-    <definedName name="Rows_SliceColumnValues">Sheet1!$E$11</definedName>
-    <definedName name="Slices">Sheet1!$E$8</definedName>
+    <definedName name="ReportTotal_SliceColumnValues">Sheet1!$C$9</definedName>
+    <definedName name="Rows">Sheet1!$A$11:$G$12</definedName>
+    <definedName name="Rows_SliceColumnValues">Sheet1!$C$11</definedName>
+    <definedName name="Slices">Sheet1!$C$8</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>Отчет по оборачиваемости с {{StartDate.ToString("dd.MM.yyyy")}} по {{EndDate.ToString("dd.MM.yyyy")}}</t>
   </si>
@@ -54,6 +54,9 @@
     <t>Дата и время формирования:  {{CreatedAt.ToString("dd.MM.yyyy HH:mm")}}</t>
   </si>
   <si>
+    <t>Периоды продаж</t>
+  </si>
+  <si>
     <t>{{item}}</t>
   </si>
   <si>
@@ -66,6 +69,9 @@
     <t>{{ShowLastSale?"Дней с последней продажи":""}}</t>
   </si>
   <si>
+    <t>{{ShowLastSale?"Остатки на складе на " + CreatedAt.ToString("dd.MM.yyyy HH:mm:ss"):""}}</t>
+  </si>
+  <si>
     <t>Сводные данные по отчету</t>
   </si>
   <si>
@@ -75,6 +81,15 @@
     <t>{{ReportTotal.LastSaleDetails != null ? ReportTotal.LastSaleDetails.DaysFromLastShipment.ToString("0") : ""}}</t>
   </si>
   <si>
+    <t>{{ReportTotal.LastSaleDetails != null ? ReportTotal.LastSaleDetails.WarhouseResidue.ToString("0") : ""}}</t>
+  </si>
+  <si>
+    <t>№</t>
+  </si>
+  <si>
+    <t>Номенклатура</t>
+  </si>
+  <si>
     <t>{{item.IsTotalsRow ? "" : item.Index}}</t>
   </si>
   <si>
@@ -90,22 +105,10 @@
     <t>{{item.LastSaleDetails != null ? item.LastSaleDetails.DaysFromLastShipment.ToString("0") : ""}}</t>
   </si>
   <si>
-    <t>Телефоны</t>
-  </si>
-  <si>
-    <t>{{item.Phones}}</t>
-  </si>
-  <si>
-    <t>E-mail</t>
-  </si>
-  <si>
-    <t>{{item.Emails}}</t>
-  </si>
-  <si>
-    <t>Группировка: {{GroupingTitle}}</t>
-  </si>
-  <si>
-    <t>{{GroupingTitle}}</t>
+    <t>{{item.LastSaleDetails != null ? item.LastSaleDetails.WarhouseResidue.ToString("0") : ""}}</t>
+  </si>
+  <si>
+    <t>Группировка: Номенклатура</t>
   </si>
 </sst>
 </file>
@@ -163,7 +166,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -189,15 +192,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -220,17 +220,7 @@
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <charset val="1"/>
-      </font>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <b/>
@@ -551,222 +541,199 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:S11"/>
+  <dimension ref="A2:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:B8"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.140625" style="3" customWidth="1"/>
     <col min="2" max="2" width="46" style="3" customWidth="1"/>
-    <col min="3" max="4" width="19.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="6.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="3" customWidth="1"/>
-    <col min="7" max="8" width="9.140625" style="3"/>
-    <col min="9" max="9" width="22.140625" style="3" customWidth="1"/>
-    <col min="10" max="14" width="9.140625" style="3"/>
-    <col min="16" max="16384" width="9.140625" style="3"/>
+    <col min="3" max="3" width="6.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="3" customWidth="1"/>
+    <col min="5" max="6" width="9.140625" style="3"/>
+    <col min="7" max="7" width="22.140625" style="3" customWidth="1"/>
+    <col min="8" max="12" width="9.140625" style="3"/>
+    <col min="14" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:19" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
-      <c r="S2" s="15"/>
-    </row>
-    <row r="3" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+    </row>
+    <row r="3" spans="1:17" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="2" t="s">
+      <c r="B3" s="15"/>
+      <c r="C3"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="46.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+    <row r="4" spans="1:17" ht="46.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="18" t="s">
+      <c r="B4" s="16"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="18"/>
-      <c r="O4" s="18"/>
-      <c r="P4" s="18"/>
-      <c r="Q4" s="18"/>
-      <c r="R4" s="18"/>
-      <c r="S4" s="18"/>
-    </row>
-    <row r="5" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="17"/>
+    </row>
+    <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="J5" s="19" t="s">
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="H5" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
-      <c r="O5" s="19"/>
-      <c r="P5" s="19"/>
-      <c r="Q5" s="19"/>
-      <c r="R5" s="19"/>
-      <c r="S5" s="19"/>
-    </row>
-    <row r="6" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="18"/>
+    </row>
+    <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+    </row>
+    <row r="8" spans="1:17" ht="49.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B9" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="9"/>
+      <c r="F9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
-      <c r="S6" s="10"/>
-    </row>
-    <row r="8" spans="1:19" ht="49.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="G11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="I8" s="7"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="9"/>
-      <c r="H9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>18</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="7">
     <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A2:S2"/>
+    <mergeCell ref="A2:Q2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
-    <mergeCell ref="G4:S4"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="J5:S5"/>
-    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="E4:Q4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="H5:Q5"/>
   </mergeCells>
-  <conditionalFormatting sqref="A11:B11 D11:F11">
-    <cfRule type="expression" dxfId="1" priority="3">
-      <formula>$A11=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C11">
-    <cfRule type="expression" dxfId="0" priority="1">
+  <conditionalFormatting sqref="A11:D11">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>$A11=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Revert "Merge branch 'master' into develop"
This reverts commit 194e1b133a31c2091528c12b1feede35a62df6ab.
</commit_message>
<xml_diff>
--- a/Source/Libraries/Core/Business/Vodovoz.Reports/Reports/Sales/TurnoverReport.xlsx
+++ b/Source/Libraries/Core/Business/Vodovoz.Reports/Reports/Sales/TurnoverReport.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rm87\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3473DB2F-0590-41B2-B501-B9D44D181174}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{701E2721-ACDE-4BC0-B762-BA047BD8D393}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3945" yWindow="4260" windowWidth="21555" windowHeight="11340" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ReportTotal_SliceColumnValues">Sheet1!$C$9</definedName>
-    <definedName name="Rows">Sheet1!$A$11:$G$12</definedName>
-    <definedName name="Rows_SliceColumnValues">Sheet1!$C$11</definedName>
-    <definedName name="Slices">Sheet1!$C$8</definedName>
+    <definedName name="ReportTotal_SliceColumnValues">Sheet1!$E$9</definedName>
+    <definedName name="Rows">Sheet1!$A$11:$I$12</definedName>
+    <definedName name="Rows_SliceColumnValues">Sheet1!$E$11</definedName>
+    <definedName name="Slices">Sheet1!$E$8</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Отчет по оборачиваемости с {{StartDate.ToString("dd.MM.yyyy")}} по {{EndDate.ToString("dd.MM.yyyy")}}</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Дата и время формирования:  {{CreatedAt.ToString("dd.MM.yyyy HH:mm")}}</t>
   </si>
   <si>
-    <t>Периоды продаж</t>
-  </si>
-  <si>
     <t>{{item}}</t>
   </si>
   <si>
@@ -69,9 +66,6 @@
     <t>{{ShowLastSale?"Дней с последней продажи":""}}</t>
   </si>
   <si>
-    <t>{{ShowLastSale?"Остатки на складе на " + CreatedAt.ToString("dd.MM.yyyy HH:mm:ss"):""}}</t>
-  </si>
-  <si>
     <t>Сводные данные по отчету</t>
   </si>
   <si>
@@ -81,15 +75,6 @@
     <t>{{ReportTotal.LastSaleDetails != null ? ReportTotal.LastSaleDetails.DaysFromLastShipment.ToString("0") : ""}}</t>
   </si>
   <si>
-    <t>{{ReportTotal.LastSaleDetails != null ? ReportTotal.LastSaleDetails.WarhouseResidue.ToString("0") : ""}}</t>
-  </si>
-  <si>
-    <t>№</t>
-  </si>
-  <si>
-    <t>Номенклатура</t>
-  </si>
-  <si>
     <t>{{item.IsTotalsRow ? "" : item.Index}}</t>
   </si>
   <si>
@@ -105,10 +90,22 @@
     <t>{{item.LastSaleDetails != null ? item.LastSaleDetails.DaysFromLastShipment.ToString("0") : ""}}</t>
   </si>
   <si>
-    <t>{{item.LastSaleDetails != null ? item.LastSaleDetails.WarhouseResidue.ToString("0") : ""}}</t>
-  </si>
-  <si>
-    <t>Группировка: Номенклатура</t>
+    <t>Телефоны</t>
+  </si>
+  <si>
+    <t>{{item.Phones}}</t>
+  </si>
+  <si>
+    <t>E-mail</t>
+  </si>
+  <si>
+    <t>{{item.Emails}}</t>
+  </si>
+  <si>
+    <t>Группировка: {{GroupingTitle}}</t>
+  </si>
+  <si>
+    <t>{{GroupingTitle}}</t>
   </si>
 </sst>
 </file>
@@ -166,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -192,12 +189,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -220,7 +220,17 @@
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -541,199 +551,222 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:Q11"/>
+  <dimension ref="A2:S11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A8" sqref="A8:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.140625" style="3" customWidth="1"/>
     <col min="2" max="2" width="46" style="3" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="3" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="3"/>
-    <col min="7" max="7" width="22.140625" style="3" customWidth="1"/>
-    <col min="8" max="12" width="9.140625" style="3"/>
-    <col min="14" max="16384" width="9.140625" style="3"/>
+    <col min="3" max="4" width="19.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="3" customWidth="1"/>
+    <col min="7" max="8" width="9.140625" style="3"/>
+    <col min="9" max="9" width="22.140625" style="3" customWidth="1"/>
+    <col min="10" max="14" width="9.140625" style="3"/>
+    <col min="16" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:19" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-    </row>
-    <row r="3" spans="1:17" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+    </row>
+    <row r="3" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="2" t="s">
+      <c r="B3" s="16"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="46.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+    <row r="4" spans="1:19" ht="46.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="17" t="s">
+      <c r="B4" s="17"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="17"/>
-    </row>
-    <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="18"/>
+      <c r="Q4" s="18"/>
+      <c r="R4" s="18"/>
+      <c r="S4" s="18"/>
+    </row>
+    <row r="5" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="H5" s="18" t="s">
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="J5" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18"/>
-      <c r="O5" s="18"/>
-      <c r="P5" s="18"/>
-      <c r="Q5" s="18"/>
-    </row>
-    <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="11"/>
-    </row>
-    <row r="8" spans="1:17" ht="49.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="19"/>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="19"/>
+      <c r="R5" s="19"/>
+      <c r="S5" s="19"/>
+    </row>
+    <row r="6" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+    </row>
+    <row r="8" spans="1:19" ht="49.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="14"/>
+      <c r="C8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="6" t="s">
+      <c r="F8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="G8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="H8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="I8" s="7"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="11" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="8" t="s">
+      <c r="G9" s="9"/>
+      <c r="H9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="12" t="s">
+      <c r="I9"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G9" t="s">
+      <c r="C11" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="11" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="G11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="H11" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A2:Q2"/>
+    <mergeCell ref="A2:S2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
-    <mergeCell ref="E4:Q4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="H5:Q5"/>
+    <mergeCell ref="G4:S4"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="J5:S5"/>
+    <mergeCell ref="A6:G6"/>
   </mergeCells>
-  <conditionalFormatting sqref="A11:D11">
-    <cfRule type="expression" dxfId="0" priority="2">
+  <conditionalFormatting sqref="A11:B11 D11:F11">
+    <cfRule type="expression" dxfId="1" priority="3">
+      <formula>$A11=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$A11=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>